<commit_message>
NIH kjørt ny passive
</commit_message>
<xml_diff>
--- a/data_output/output for F24 stiff 2018-02-12/all_stiff_output_20180212_1334 GM.xlsx
+++ b/data_output/output for F24 stiff 2018-02-12/all_stiff_output_20180212_1334 GM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\My Documents\MATLAB\tend_stiff_2\data_output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\My Documents\MATLAB\tend_stiff_2\data_output\output for F24 stiff 2018-02-12\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -153,8 +153,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -182,8 +190,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,8 +475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:AJ89"/>
+    <sheetView tabSelected="1" topLeftCell="C19" workbookViewId="0">
+      <selection activeCell="L41" sqref="L41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4793,10 +4802,10 @@
       <c r="J40">
         <v>0.9995866975105866</v>
       </c>
-      <c r="K40">
+      <c r="K40" s="1">
         <v>1800</v>
       </c>
-      <c r="L40">
+      <c r="L40" s="1">
         <v>2019.9772466778345</v>
       </c>
       <c r="M40">
@@ -4894,7 +4903,7 @@
       <c r="J41">
         <v>0.99952073309535538</v>
       </c>
-      <c r="K41">
+      <c r="K41" s="1">
         <v>1800</v>
       </c>
       <c r="L41">
@@ -10254,6 +10263,19 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="J2:J89">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>